<commit_message>
Update Model_Parameters Store model.xlsx
</commit_message>
<xml_diff>
--- a/STORE_model/Model_Parameters Store model.xlsx
+++ b/STORE_model/Model_Parameters Store model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oweisberg\Documents\GitHub\recycle_model\STORE_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9CB1AB-86AF-49E1-92E0-01400EC491E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B321C23-0AF9-474B-ABEE-6C0904C54E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -861,8 +861,8 @@
   <dimension ref="A1:R58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M61" sqref="M61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2457,7 +2457,7 @@
         <v>0.1427507995452611</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M32" s="5" t="s">
         <v>66</v>
@@ -2577,7 +2577,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M34" s="5" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
reduce Qp to 12.5 fg N/cell
</commit_message>
<xml_diff>
--- a/STORE_model/Model_Parameters Store model.xlsx
+++ b/STORE_model/Model_Parameters Store model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oweisberg\Documents\GitHub\recycle_model\STORE_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\STORE_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B321C23-0AF9-474B-ABEE-6C0904C54E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F431F70C-A45C-4266-B354-9C51F142C6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -861,8 +861,8 @@
   <dimension ref="A1:R58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M61" sqref="M61"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1136,7 +1136,7 @@
         <v>76</v>
       </c>
       <c r="E6" s="5">
-        <v>7</v>
+        <v>6.625</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1170,7 +1170,7 @@
         <v>75</v>
       </c>
       <c r="E7" s="11">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>

</xml_diff>

<commit_message>
make gamma log bounded
</commit_message>
<xml_diff>
--- a/STORE_model/Model_Parameters Store model.xlsx
+++ b/STORE_model/Model_Parameters Store model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\STORE_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oweisberg\Documents\GitHub\recycle_model\STORE_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F431F70C-A45C-4266-B354-9C51F142C6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCA2F15-60E0-40AA-9F48-4363C2695184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -862,7 +862,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="P3" sqref="P3:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1069,7 +1069,7 @@
         <v>0.9</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q4" s="5">
         <v>0.1</v>
@@ -1113,7 +1113,7 @@
         <v>0.9</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q5" s="5">
         <v>0.1</v>

</xml_diff>

<commit_message>
change the allowed limits for Mp, vmaxINp, vmaxICp to multiply by 10
</commit_message>
<xml_diff>
--- a/STORE_model/Model_Parameters Store model.xlsx
+++ b/STORE_model/Model_Parameters Store model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oweisberg\Documents\GitHub\recycle_model\STORE_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2844B4-B7EB-4134-8658-6887C572F649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFF8139-AC00-41C7-894E-49FC19E10C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -862,7 +862,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1021,8 +1021,8 @@
         <v>2.314814814814814E-7</v>
       </c>
       <c r="O3" s="4">
-        <f>E3*5</f>
-        <v>5.7870370370370351E-6</v>
+        <f>E3*10</f>
+        <v>1.157407407407407E-5</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>67</v>
@@ -1769,13 +1769,13 @@
       <c r="M19" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="N19" s="5">
-        <f t="shared" si="2"/>
-        <v>7.6467122800187402E-6</v>
-      </c>
-      <c r="O19" s="5">
-        <f t="shared" si="3"/>
-        <v>1.9116780700046852E-4</v>
+      <c r="N19" s="4">
+        <f>E19/10</f>
+        <v>3.8233561400093701E-6</v>
+      </c>
+      <c r="O19" s="4">
+        <f>E19*10</f>
+        <v>3.8233561400093704E-4</v>
       </c>
       <c r="P19" s="5" t="s">
         <v>67</v>
@@ -1877,13 +1877,13 @@
       <c r="M21" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="N21" s="5">
-        <f t="shared" si="2"/>
-        <v>5.3526985960131182E-5</v>
-      </c>
-      <c r="O21" s="5">
-        <f t="shared" si="3"/>
-        <v>1.3381746490032794E-3</v>
+      <c r="N21" s="4">
+        <f>E21/10</f>
+        <v>2.6763492980065591E-5</v>
+      </c>
+      <c r="O21" s="4">
+        <f>E21*10</f>
+        <v>2.6763492980065588E-3</v>
       </c>
       <c r="P21" s="5" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
new overflow + DON2DIN model
</commit_message>
<xml_diff>
--- a/STORE_model/Model_Parameters Store model.xlsx
+++ b/STORE_model/Model_Parameters Store model.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oweisberg\Documents\GitHub\recycle_model\STORE_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\STORE_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFF8139-AC00-41C7-894E-49FC19E10C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35DF415-F85F-4893-A953-A228F0FC296A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="129">
   <si>
     <t>Mh</t>
   </si>
@@ -348,12 +348,6 @@
     <t>Kmtbp</t>
   </si>
   <si>
-    <t>gamma_DON2DINp</t>
-  </si>
-  <si>
-    <t>gamma_DON2DINh</t>
-  </si>
-  <si>
     <t>1/ umolN/L /s</t>
   </si>
   <si>
@@ -421,6 +415,15 @@
   </si>
   <si>
     <t>omegaH</t>
+  </si>
+  <si>
+    <t>gamma_DON2DINexop</t>
+  </si>
+  <si>
+    <t>gamma_DON2DINexoh</t>
+  </si>
+  <si>
+    <t>gamma_DON2DIN</t>
   </si>
 </sst>
 </file>
@@ -858,11 +861,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R58"/>
+  <dimension ref="A1:R59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -903,16 +906,16 @@
         <v>71</v>
       </c>
       <c r="H1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="17" t="s">
         <v>108</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>110</v>
       </c>
       <c r="L1" s="16" t="s">
         <v>73</v>
@@ -1192,7 +1195,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>40</v>
@@ -1210,13 +1213,21 @@
         <f t="shared" si="0"/>
         <v>9.999999999999995E-2</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
       <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0</v>
+      </c>
       <c r="L8" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>66</v>
@@ -1241,7 +1252,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>40</v>
@@ -1259,16 +1270,24 @@
         <f t="shared" si="0"/>
         <v>9.999999999999995E-2</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
       <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0</v>
+      </c>
       <c r="L9" s="5" t="s">
         <v>66</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N9" s="4">
         <f>E9/10</f>
@@ -1375,11 +1394,11 @@
         <v>66</v>
       </c>
       <c r="N11" s="5">
-        <f t="shared" ref="N11:N21" si="2">E11/5</f>
+        <f t="shared" ref="N11:N20" si="2">E11/5</f>
         <v>2.8550159909052221E-2</v>
       </c>
       <c r="O11" s="5">
-        <f t="shared" ref="O11:O21" si="3">E11*5</f>
+        <f t="shared" ref="O11:O20" si="3">E11*5</f>
         <v>0.71375399772630543</v>
       </c>
       <c r="P11" s="5" t="s">
@@ -2084,7 +2103,7 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>47</v>
@@ -3216,7 +3235,7 @@
     </row>
     <row r="49" spans="1:18">
       <c r="A49" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>40</v>
@@ -3253,13 +3272,13 @@
     </row>
     <row r="50" spans="1:18">
       <c r="A50" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B50" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="C50" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>76</v>
@@ -3307,13 +3326,13 @@
     </row>
     <row r="51" spans="1:18">
       <c r="A51" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>75</v>
@@ -3360,53 +3379,73 @@
     </row>
     <row r="52" spans="1:18">
       <c r="A52" s="12" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D52" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E52" s="13">
-        <v>10</v>
-      </c>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
+      <c r="E52" s="4">
+        <f>1.15740740740741E-07/5</f>
+        <v>2.3148148148148201E-8</v>
+      </c>
+      <c r="F52" s="5">
+        <f t="shared" ref="F52" si="22">E52*3600*24</f>
+        <v>2.0000000000000044E-3</v>
+      </c>
+      <c r="G52" s="5">
+        <v>0</v>
+      </c>
+      <c r="H52" s="5">
+        <v>0</v>
+      </c>
       <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
+      <c r="J52" s="5">
+        <v>0</v>
+      </c>
+      <c r="K52" s="5">
+        <v>0</v>
+      </c>
       <c r="L52" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M52" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-      <c r="P52" s="5"/>
+      <c r="N52" s="5">
+        <f t="shared" ref="N52" si="23">E52/5</f>
+        <v>4.6296296296296403E-9</v>
+      </c>
+      <c r="O52" s="5">
+        <f t="shared" ref="O52" si="24">E52*5</f>
+        <v>1.1574074074074101E-7</v>
+      </c>
+      <c r="P52" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="Q52" s="5"/>
       <c r="R52" s="5"/>
     </row>
     <row r="53" spans="1:18">
       <c r="A53" s="12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E53" s="13">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
@@ -3428,19 +3467,19 @@
     </row>
     <row r="54" spans="1:18">
       <c r="A54" s="12" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E54" s="13">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
@@ -3462,19 +3501,19 @@
     </row>
     <row r="55" spans="1:18">
       <c r="A55" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>75</v>
       </c>
       <c r="E55" s="13">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
@@ -3495,37 +3534,27 @@
       <c r="R55" s="5"/>
     </row>
     <row r="56" spans="1:18">
-      <c r="A56" s="20" t="s">
-        <v>122</v>
+      <c r="A56" s="12" t="s">
+        <v>118</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E56" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F56" s="5"/>
-      <c r="G56" s="5">
-        <v>0</v>
-      </c>
-      <c r="H56" s="5">
-        <v>0</v>
-      </c>
-      <c r="I56" s="5">
-        <v>0</v>
-      </c>
-      <c r="J56" s="5">
-        <v>1</v>
-      </c>
-      <c r="K56" s="5">
-        <v>0</v>
-      </c>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
       <c r="L56" s="5" t="s">
         <v>66</v>
       </c>
@@ -3539,20 +3568,20 @@
       <c r="R56" s="5"/>
     </row>
     <row r="57" spans="1:18">
-      <c r="A57" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E57" s="5">
-        <v>0.01</v>
+      <c r="A57" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E57" s="13">
+        <v>1</v>
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="5">
@@ -3564,49 +3593,39 @@
       <c r="I57" s="5">
         <v>0</v>
       </c>
-      <c r="J57" s="5"/>
+      <c r="J57" s="5">
+        <v>1</v>
+      </c>
       <c r="K57" s="5">
         <v>0</v>
       </c>
       <c r="L57" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M57" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="N57" s="4">
-        <f t="shared" ref="N57:N58" si="22">E57/10</f>
-        <v>1E-3</v>
-      </c>
-      <c r="O57" s="4">
-        <f t="shared" ref="O57:O58" si="23">E57*10</f>
-        <v>0.1</v>
-      </c>
-      <c r="P57" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q57" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="R57" s="5">
-        <v>0.1</v>
-      </c>
+      <c r="N57" s="5"/>
+      <c r="O57" s="5"/>
+      <c r="P57" s="5"/>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="5"/>
     </row>
     <row r="58" spans="1:18">
       <c r="A58" s="18" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E58" s="5">
-        <v>1.0000000000000001E-5</v>
+        <v>0.01</v>
       </c>
       <c r="F58" s="5"/>
       <c r="G58" s="5">
@@ -3623,31 +3642,85 @@
         <v>0</v>
       </c>
       <c r="L58" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M58" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N58" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="N58:N59" si="25">E58/10</f>
+        <v>1E-3</v>
+      </c>
+      <c r="O58" s="4">
+        <f t="shared" ref="O58:O59" si="26">E58*10</f>
+        <v>0.1</v>
+      </c>
+      <c r="P58" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q58" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="R58" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18">
+      <c r="A59" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E59" s="5">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5">
+        <v>0</v>
+      </c>
+      <c r="H59" s="5">
+        <v>0</v>
+      </c>
+      <c r="I59" s="5">
+        <v>0</v>
+      </c>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5">
+        <v>0</v>
+      </c>
+      <c r="L59" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="M59" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N59" s="4">
+        <f t="shared" si="25"/>
         <v>1.0000000000000002E-6</v>
       </c>
-      <c r="O58" s="4">
-        <f t="shared" si="23"/>
+      <c r="O59" s="4">
+        <f t="shared" si="26"/>
         <v>1E-4</v>
       </c>
-      <c r="P58" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q58" s="5">
+      <c r="P59" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q59" s="5">
         <v>1.0000000000000002E-6</v>
       </c>
-      <c r="R58" s="5">
+      <c r="R59" s="5">
         <v>1E-4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R58" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:R59" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
DON2DIN for all models
</commit_message>
<xml_diff>
--- a/STORE_model/Model_Parameters Store model.xlsx
+++ b/STORE_model/Model_Parameters Store model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\STORE_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35DF415-F85F-4893-A953-A228F0FC296A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC52A22-8FDC-4BB1-A846-3BDBEABD4872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="129">
   <si>
     <t>Mh</t>
   </si>
@@ -864,8 +864,8 @@
   <dimension ref="A1:R59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3398,36 +3398,20 @@
         <f t="shared" ref="F52" si="22">E52*3600*24</f>
         <v>2.0000000000000044E-3</v>
       </c>
-      <c r="G52" s="5">
-        <v>0</v>
-      </c>
-      <c r="H52" s="5">
-        <v>0</v>
-      </c>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
       <c r="I52" s="5"/>
-      <c r="J52" s="5">
-        <v>0</v>
-      </c>
-      <c r="K52" s="5">
-        <v>0</v>
-      </c>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
       <c r="L52" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M52" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="N52" s="5">
-        <f t="shared" ref="N52" si="23">E52/5</f>
-        <v>4.6296296296296403E-9</v>
-      </c>
-      <c r="O52" s="5">
-        <f t="shared" ref="O52" si="24">E52*5</f>
-        <v>1.1574074074074101E-7</v>
-      </c>
-      <c r="P52" s="5" t="s">
-        <v>67</v>
-      </c>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+      <c r="P52" s="5"/>
       <c r="Q52" s="5"/>
       <c r="R52" s="5"/>
     </row>
@@ -3648,11 +3632,11 @@
         <v>66</v>
       </c>
       <c r="N58" s="4">
-        <f t="shared" ref="N58:N59" si="25">E58/10</f>
+        <f t="shared" ref="N58:N59" si="23">E58/10</f>
         <v>1E-3</v>
       </c>
       <c r="O58" s="4">
-        <f t="shared" ref="O58:O59" si="26">E58*10</f>
+        <f t="shared" ref="O58:O59" si="24">E58*10</f>
         <v>0.1</v>
       </c>
       <c r="P58" s="5" t="s">
@@ -3702,11 +3686,11 @@
         <v>67</v>
       </c>
       <c r="N59" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>1.0000000000000002E-6</v>
       </c>
       <c r="O59" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>1E-4</v>
       </c>
       <c r="P59" s="5" t="s">

</xml_diff>

<commit_message>
C specific C vmax + bugfixes
</commit_message>
<xml_diff>
--- a/STORE_model/Model_Parameters Store model.xlsx
+++ b/STORE_model/Model_Parameters Store model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\STORE_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A0AF0A-0F9D-49F3-8027-1D3E34ABBA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC972FF-2D88-4788-B237-9F5D307A65CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,13 +376,13 @@
 d-1</t>
   </si>
   <si>
-    <t>paramROSmaxD</t>
-  </si>
-  <si>
     <t>max ROS toxicity (additional death)</t>
   </si>
   <si>
     <t xml:space="preserve">s-1 </t>
+  </si>
+  <si>
+    <t>ROSmaxD</t>
   </si>
 </sst>
 </file>
@@ -550,7 +550,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
@@ -863,7 +863,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
+      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2969,19 +2969,19 @@
     </row>
     <row r="48" spans="1:17">
       <c r="A48" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B48" s="21">
         <v>3.2055555555555556E-5</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>77</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
update vmax ICP (following sensitivity)
</commit_message>
<xml_diff>
--- a/STORE_model/Model_Parameters Store model.xlsx
+++ b/STORE_model/Model_Parameters Store model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\STORE_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC972FF-2D88-4788-B237-9F5D307A65CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2203994A-1A5E-4F45-912C-BBBBC9757A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -860,10 +860,10 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -940,14 +940,14 @@
         <v>17</v>
       </c>
       <c r="B2" s="13">
-        <v>2.2315471698113204E-6</v>
+        <v>5.5555555555555558E-6</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>83</v>
       </c>
       <c r="D2" s="15">
         <f t="shared" ref="D2:D9" si="0">B2*3600*24</f>
-        <v>0.19280567547169808</v>
+        <v>0.48</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>52</v>
@@ -971,11 +971,11 @@
       </c>
       <c r="O2" s="13">
         <f>B2/10</f>
-        <v>2.2315471698113204E-7</v>
+        <v>5.5555555555555562E-7</v>
       </c>
       <c r="P2" s="13">
         <f>B2*10</f>
-        <v>2.2315471698113206E-5</v>
+        <v>5.5555555555555558E-5</v>
       </c>
       <c r="Q2" s="8" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
increase vmaxONp and vmaxOCp following discussion with Daniel
</commit_message>
<xml_diff>
--- a/STORE_model/Model_Parameters Store model.xlsx
+++ b/STORE_model/Model_Parameters Store model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\STORE_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2203994A-1A5E-4F45-912C-BBBBC9757A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD9676D-4D54-4023-9CCB-5CB6AE20450A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -427,12 +427,18 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -501,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -553,6 +559,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,7 +885,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1116,14 +1138,14 @@
         <v>16</v>
       </c>
       <c r="B6" s="13">
-        <v>2.7049056603773586E-8</v>
+        <v>1.8518518518518519E-6</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="15">
         <f t="shared" si="0"/>
-        <v>2.3370384905660379E-3</v>
+        <v>0.16</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>52</v>
@@ -1155,59 +1177,59 @@
       </c>
       <c r="O6" s="13">
         <f t="shared" si="1"/>
-        <v>2.7049056603773586E-9</v>
+        <v>1.8518518518518518E-7</v>
       </c>
       <c r="P6" s="13">
         <f t="shared" si="2"/>
-        <v>2.7049056603773587E-7</v>
+        <v>1.8518518518518518E-5</v>
       </c>
       <c r="Q6" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:17" s="30" customFormat="1">
+      <c r="A7" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="24">
         <v>5.5416666666666663E-8</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="26">
         <f t="shared" si="0"/>
         <v>4.7879999999999997E-3</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="O7" s="13">
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="O7" s="24">
         <f t="shared" si="1"/>
         <v>5.5416666666666667E-9</v>
       </c>
-      <c r="P7" s="13">
-        <f t="shared" si="2"/>
-        <v>5.5416666666666662E-7</v>
-      </c>
-      <c r="Q7" s="8" t="s">
+      <c r="P7" s="24">
+        <f>B7*10000</f>
+        <v>5.5416666666666667E-4</v>
+      </c>
+      <c r="Q7" s="29" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1216,14 +1238,14 @@
         <v>14</v>
       </c>
       <c r="B8" s="13">
-        <v>1.0888888888888888E-7</v>
+        <v>1.1111111111111112E-6</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>83</v>
       </c>
       <c r="D8" s="15">
         <f t="shared" si="0"/>
-        <v>9.407999999999998E-3</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>52</v>
@@ -1255,11 +1277,11 @@
       </c>
       <c r="O8" s="13">
         <f t="shared" si="1"/>
-        <v>1.0888888888888888E-8</v>
+        <v>1.1111111111111112E-7</v>
       </c>
       <c r="P8" s="13">
         <f t="shared" si="2"/>
-        <v>1.0888888888888889E-6</v>
+        <v>1.1111111111111112E-5</v>
       </c>
       <c r="Q8" s="8" t="s">
         <v>43</v>
@@ -1304,8 +1326,8 @@
         <v>4.2777777777777778E-9</v>
       </c>
       <c r="P9" s="13">
-        <f t="shared" si="2"/>
-        <v>4.2777777777777781E-7</v>
+        <f>B9*1000</f>
+        <v>4.2777777777777778E-5</v>
       </c>
       <c r="Q9" s="8" t="s">
         <v>43</v>
@@ -2098,14 +2120,15 @@
         <v>57</v>
       </c>
       <c r="B29" s="13">
-        <v>3.4999999999999997E-5</v>
+        <f>B28*5</f>
+        <v>1.7499999999999997E-4</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>83</v>
       </c>
       <c r="D29" s="8">
         <f>B29*3600*24</f>
-        <v>3.024</v>
+        <v>15.119999999999997</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>51</v>
@@ -3006,7 +3029,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q47" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:Q48" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A39:Q40">
       <sortCondition ref="A1:A47"/>
     </sortState>

</xml_diff>

<commit_message>
update het uptake rates
</commit_message>
<xml_diff>
--- a/STORE_model/Model_Parameters Store model.xlsx
+++ b/STORE_model/Model_Parameters Store model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\STORE_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD9676D-4D54-4023-9CCB-5CB6AE20450A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED40394-7C09-497F-9E4A-3B769FE4F286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,18 +427,12 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -559,22 +553,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -882,10 +876,10 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1092,14 +1086,14 @@
         <v>19</v>
       </c>
       <c r="B5" s="13">
-        <v>1.6666666666666667E-6</v>
+        <v>6.666666666666667E-5</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>83</v>
       </c>
       <c r="D5" s="15">
         <f t="shared" si="0"/>
-        <v>0.14400000000000002</v>
+        <v>5.7600000000000007</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>51</v>
@@ -1123,11 +1117,11 @@
       </c>
       <c r="O5" s="13">
         <f t="shared" si="1"/>
-        <v>1.6666666666666668E-7</v>
+        <v>6.6666666666666666E-6</v>
       </c>
       <c r="P5" s="13">
         <f t="shared" si="2"/>
-        <v>1.6666666666666667E-5</v>
+        <v>6.6666666666666675E-4</v>
       </c>
       <c r="Q5" s="8" t="s">
         <v>43</v>
@@ -1192,14 +1186,14 @@
         <v>20</v>
       </c>
       <c r="B7" s="24">
-        <v>5.5416666666666663E-8</v>
+        <v>6.666666666666667E-5</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>83</v>
       </c>
       <c r="D7" s="26">
         <f t="shared" si="0"/>
-        <v>4.7879999999999997E-3</v>
+        <v>5.7600000000000007</v>
       </c>
       <c r="E7" s="27" t="s">
         <v>51</v>
@@ -1223,11 +1217,11 @@
       </c>
       <c r="O7" s="24">
         <f t="shared" si="1"/>
-        <v>5.5416666666666667E-9</v>
+        <v>6.6666666666666666E-6</v>
       </c>
       <c r="P7" s="24">
-        <f>B7*10000</f>
-        <v>5.5416666666666667E-4</v>
+        <f>B7*10</f>
+        <v>6.6666666666666675E-4</v>
       </c>
       <c r="Q7" s="29" t="s">
         <v>43</v>
@@ -1292,14 +1286,14 @@
         <v>18</v>
       </c>
       <c r="B9" s="13">
-        <v>4.2777777777777779E-8</v>
+        <v>6.666666666666667E-5</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>83</v>
       </c>
       <c r="D9" s="16">
         <f t="shared" si="0"/>
-        <v>3.6960000000000001E-3</v>
+        <v>5.7600000000000007</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>51</v>
@@ -1323,11 +1317,11 @@
       </c>
       <c r="O9" s="13">
         <f t="shared" si="1"/>
-        <v>4.2777777777777778E-9</v>
+        <v>6.6666666666666666E-6</v>
       </c>
       <c r="P9" s="13">
-        <f>B9*1000</f>
-        <v>4.2777777777777778E-5</v>
+        <f>B9*10</f>
+        <v>6.6666666666666675E-4</v>
       </c>
       <c r="Q9" s="8" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
add 3 models combinations
</commit_message>
<xml_diff>
--- a/STORE_model/Model_Parameters Store model.xlsx
+++ b/STORE_model/Model_Parameters Store model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oweisberg\Documents\GitHub\recycle_model\STORE_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\STORE_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2489E8B-4C43-4F96-882C-7AD4711B647E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D08425D-3E1C-4347-952F-9E685FC174C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$X$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AB$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="145">
   <si>
     <t>Mh</t>
   </si>
@@ -386,27 +386,6 @@
     <t>ROSmaxD</t>
   </si>
   <si>
-    <t>OVERFLOW_EXOENZYME model hardcoded parameters</t>
-  </si>
-  <si>
-    <t>OVERFLOW_ROS model hardcoded parameters</t>
-  </si>
-  <si>
-    <t>OVERFLOW_MIXOTROPH model hardcoded parameters</t>
-  </si>
-  <si>
-    <t>EXOENZYME_ROS model hardcoded parameters</t>
-  </si>
-  <si>
-    <t>EXOENZYME_MIXOTROPH model hardcoded parameters</t>
-  </si>
-  <si>
-    <t>ROS_MIXOTROPH model hardcoded parameters</t>
-  </si>
-  <si>
-    <t>ROS_MIXOTROPH_OVERFLOW_EXOENZYME model hardcoded parameters</t>
-  </si>
-  <si>
     <t>MIN</t>
   </si>
   <si>
@@ -429,6 +408,72 @@
   </si>
   <si>
     <t>OVERFLOW_ROS</t>
+  </si>
+  <si>
+    <t>ROS-MIXOTROPH-OVERFLOW-EXOENZYME model hardcoded parameters</t>
+  </si>
+  <si>
+    <t>ROS-MIXOTROPH model hardcoded parameters</t>
+  </si>
+  <si>
+    <t>EXOENZYME-ROS model hardcoded parameters</t>
+  </si>
+  <si>
+    <t>EXOENZYME-MIXOTROPH model hardcoded parameters</t>
+  </si>
+  <si>
+    <t>OVERFLOW-MIXOTROPH model hardcoded parameters</t>
+  </si>
+  <si>
+    <t>OVERFLOW-EXOENZYME model hardcoded parameters</t>
+  </si>
+  <si>
+    <t>OVERFLOW-ROS model hardcoded parameters</t>
+  </si>
+  <si>
+    <t>OVERFLOW-ROS-EXOENZYME model hardcoded parameters</t>
+  </si>
+  <si>
+    <t>OVERFLOW-ROS-MIXOTROPH model hardcoded parameters</t>
+  </si>
+  <si>
+    <t>OVERFLOW-EXOENZYME-MIXOTROPH model hardcoded parameters</t>
+  </si>
+  <si>
+    <t>EXOENZYME-ROS-MIXOTROPH model hardcoded parameters</t>
+  </si>
+  <si>
+    <t>ROS-MIXOTROPH-OVERFLOW-EXOENZYME</t>
+  </si>
+  <si>
+    <t>ROS-MIXOTROPH</t>
+  </si>
+  <si>
+    <t>EXOENZYME-ROS</t>
+  </si>
+  <si>
+    <t>EXOENZYME-MIXOTROPH</t>
+  </si>
+  <si>
+    <t>OVERFLOW-MIXOTROPH</t>
+  </si>
+  <si>
+    <t>OVERFLOW-EXOENZYME</t>
+  </si>
+  <si>
+    <t>OVERFLOW-ROS</t>
+  </si>
+  <si>
+    <t>EXOENZYME-ROS-MIXOTROPH</t>
+  </si>
+  <si>
+    <t>OVERFLOW-EXOENZYME-MIXOTROPH</t>
+  </si>
+  <si>
+    <t>OVERFLOW-ROS-MIXOTROPH</t>
+  </si>
+  <si>
+    <t>OVERFLOW-ROS-EXOENZYME</t>
   </si>
 </sst>
 </file>
@@ -602,11 +647,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -911,13 +956,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X48"/>
+  <dimension ref="A1:AB48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -932,12 +977,12 @@
     <col min="8" max="8" width="13.140625" customWidth="1"/>
     <col min="9" max="11" width="14.42578125" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="19" width="14.42578125" customWidth="1"/>
-    <col min="20" max="21" width="12.85546875" customWidth="1"/>
-    <col min="22" max="24" width="9.140625" customWidth="1"/>
+    <col min="13" max="23" width="14.42578125" customWidth="1"/>
+    <col min="24" max="25" width="12.85546875" customWidth="1"/>
+    <col min="26" max="28" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="3" customFormat="1" ht="90">
+    <row r="1" spans="1:28" s="3" customFormat="1" ht="105">
       <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
@@ -975,43 +1020,55 @@
         <v>60</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="T1" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="W1" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="X1" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="Y1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="Z1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="AA1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="AB1" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:28">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
@@ -1046,25 +1103,29 @@
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V2" s="13">
+      <c r="Z2" s="13">
         <f>B2/10</f>
         <v>5.5555555555555562E-7</v>
       </c>
-      <c r="W2" s="13">
+      <c r="AA2" s="13">
         <f>B2*10</f>
         <v>5.5555555555555558E-5</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="AB2" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:28">
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
@@ -1099,17 +1160,21 @@
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
-      <c r="T3" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="X3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:28">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -1144,25 +1209,29 @@
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="U4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="V4" s="13">
-        <f t="shared" ref="V4:V10" si="1">B4/10</f>
-        <v>5.5555555555555562E-7</v>
-      </c>
-      <c r="W4" s="13">
-        <f t="shared" ref="W4:W10" si="2">B4*10</f>
-        <v>5.5555555555555558E-5</v>
-      </c>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
       <c r="X4" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="Y4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z4" s="13">
+        <f t="shared" ref="Z4:Z10" si="1">B4/10</f>
+        <v>5.5555555555555562E-7</v>
+      </c>
+      <c r="AA4" s="13">
+        <f t="shared" ref="AA4:AA10" si="2">B4*10</f>
+        <v>5.5555555555555558E-5</v>
+      </c>
+      <c r="AB4" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28">
       <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
@@ -1197,25 +1266,29 @@
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
-      <c r="T5" s="8" t="s">
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U5" s="8" t="s">
+      <c r="Y5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="V5" s="13">
+      <c r="Z5" s="13">
         <f t="shared" si="1"/>
         <v>6.6666666666666666E-6</v>
       </c>
-      <c r="W5" s="13">
+      <c r="AA5" s="13">
         <f t="shared" si="2"/>
         <v>6.6666666666666675E-4</v>
       </c>
-      <c r="X5" s="8" t="s">
+      <c r="AB5" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:28">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
@@ -1264,25 +1337,31 @@
       <c r="S6" s="8">
         <v>0</v>
       </c>
-      <c r="T6" s="8" t="s">
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8">
+        <v>0</v>
+      </c>
+      <c r="X6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U6" s="8" t="s">
+      <c r="Y6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V6" s="13">
+      <c r="Z6" s="13">
         <f t="shared" si="1"/>
         <v>1.8518518518518518E-7</v>
       </c>
-      <c r="W6" s="13">
+      <c r="AA6" s="13">
         <f t="shared" si="2"/>
         <v>1.8518518518518518E-5</v>
       </c>
-      <c r="X6" s="8" t="s">
+      <c r="AB6" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:28">
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
@@ -1317,25 +1396,29 @@
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
-      <c r="T7" s="8" t="s">
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U7" s="8" t="s">
+      <c r="Y7" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="V7" s="13">
+      <c r="Z7" s="13">
         <f t="shared" si="1"/>
         <v>6.6666666666666666E-6</v>
       </c>
-      <c r="W7" s="13">
+      <c r="AA7" s="13">
         <f>B7*10</f>
         <v>6.6666666666666675E-4</v>
       </c>
-      <c r="X7" s="8" t="s">
+      <c r="AB7" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:28">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -1384,25 +1467,31 @@
       <c r="S8" s="8">
         <v>0</v>
       </c>
-      <c r="T8" s="8" t="s">
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8">
+        <v>0</v>
+      </c>
+      <c r="X8" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U8" s="8" t="s">
+      <c r="Y8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V8" s="13">
+      <c r="Z8" s="13">
         <f t="shared" si="1"/>
         <v>1.1111111111111112E-7</v>
       </c>
-      <c r="W8" s="13">
+      <c r="AA8" s="13">
         <f t="shared" si="2"/>
         <v>1.1111111111111112E-5</v>
       </c>
-      <c r="X8" s="8" t="s">
+      <c r="AB8" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:28">
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
@@ -1437,25 +1526,29 @@
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
-      <c r="T9" s="8" t="s">
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U9" s="8" t="s">
+      <c r="Y9" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="V9" s="13">
+      <c r="Z9" s="13">
         <f t="shared" si="1"/>
         <v>6.6666666666666666E-6</v>
       </c>
-      <c r="W9" s="13">
+      <c r="AA9" s="13">
         <f>B9*10</f>
         <v>6.6666666666666675E-4</v>
       </c>
-      <c r="X9" s="8" t="s">
+      <c r="AB9" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:28">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
@@ -1487,25 +1580,29 @@
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
       <c r="S10" s="8"/>
-      <c r="T10" s="8" t="s">
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U10" s="8" t="s">
+      <c r="Y10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V10" s="8">
+      <c r="Z10" s="8">
         <f t="shared" si="1"/>
         <v>3.7</v>
       </c>
-      <c r="W10" s="8">
+      <c r="AA10" s="8">
         <f t="shared" si="2"/>
         <v>370</v>
       </c>
-      <c r="X10" s="8" t="s">
+      <c r="AB10" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:28">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -1537,17 +1634,21 @@
       <c r="Q11" s="15"/>
       <c r="R11" s="15"/>
       <c r="S11" s="15"/>
-      <c r="T11" s="8" t="s">
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U11" s="8" t="s">
+      <c r="Y11" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-    </row>
-    <row r="12" spans="1:24">
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+    </row>
+    <row r="12" spans="1:28">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
@@ -1579,25 +1680,29 @@
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
       <c r="S12" s="8"/>
-      <c r="T12" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="U12" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="V12" s="8">
-        <f t="shared" ref="V12:V19" si="3">B12/10</f>
-        <v>2E-3</v>
-      </c>
-      <c r="W12" s="8">
-        <f t="shared" ref="W12:W19" si="4">B12*10</f>
-        <v>0.2</v>
-      </c>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
       <c r="X12" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:24">
+      <c r="Y12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z12" s="8">
+        <f t="shared" ref="Z12:Z19" si="3">B12/10</f>
+        <v>2E-3</v>
+      </c>
+      <c r="AA12" s="8">
+        <f t="shared" ref="AA12:AA19" si="4">B12*10</f>
+        <v>0.2</v>
+      </c>
+      <c r="AB12" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28">
       <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
@@ -1629,25 +1734,29 @@
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
-      <c r="T13" s="8" t="s">
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U13" s="8" t="s">
+      <c r="Y13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="V13" s="13">
+      <c r="Z13" s="13">
         <f t="shared" si="3"/>
         <v>2E-3</v>
       </c>
-      <c r="W13" s="13">
+      <c r="AA13" s="13">
         <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
-      <c r="X13" s="8" t="s">
+      <c r="AB13" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:28">
       <c r="A14" s="6" t="s">
         <v>8</v>
       </c>
@@ -1700,25 +1809,32 @@
         <f>$B14</f>
         <v>0.03</v>
       </c>
-      <c r="T14" s="8" t="s">
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15">
+        <f>$B14</f>
+        <v>0.03</v>
+      </c>
+      <c r="X14" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U14" s="8" t="s">
+      <c r="Y14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V14" s="8">
+      <c r="Z14" s="8">
         <f t="shared" si="3"/>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="W14" s="8">
+      <c r="AA14" s="8">
         <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
-      <c r="X14" s="8" t="s">
+      <c r="AB14" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:28">
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
@@ -1750,25 +1866,29 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
-      <c r="T15" s="8" t="s">
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U15" s="8" t="s">
+      <c r="Y15" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="V15" s="13">
+      <c r="Z15" s="13">
         <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
-      <c r="W15" s="13">
+      <c r="AA15" s="13">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="X15" s="8" t="s">
+      <c r="AB15" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:28">
       <c r="A16" s="6" t="s">
         <v>6</v>
       </c>
@@ -1821,25 +1941,32 @@
         <f>$B16</f>
         <v>0.1</v>
       </c>
-      <c r="T16" s="8" t="s">
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15">
+        <f>$B16</f>
+        <v>0.1</v>
+      </c>
+      <c r="X16" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U16" s="8" t="s">
+      <c r="Y16" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V16" s="8">
+      <c r="Z16" s="8">
         <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
-      <c r="W16" s="8">
+      <c r="AA16" s="8">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="X16" s="8" t="s">
+      <c r="AB16" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:28">
       <c r="A17" s="6" t="s">
         <v>10</v>
       </c>
@@ -1871,25 +1998,29 @@
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
-      <c r="T17" s="8" t="s">
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U17" s="8" t="s">
+      <c r="Y17" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="V17" s="13">
+      <c r="Z17" s="13">
         <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
-      <c r="W17" s="13">
+      <c r="AA17" s="13">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="X17" s="8" t="s">
+      <c r="AB17" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:28">
       <c r="A18" s="6" t="s">
         <v>1</v>
       </c>
@@ -1924,25 +2055,29 @@
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
-      <c r="T18" s="8" t="s">
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U18" s="8" t="s">
+      <c r="Y18" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V18" s="13">
+      <c r="Z18" s="13">
         <f t="shared" si="3"/>
         <v>1.157407407407407E-7</v>
       </c>
-      <c r="W18" s="13">
+      <c r="AA18" s="13">
         <f t="shared" si="4"/>
         <v>1.157407407407407E-5</v>
       </c>
-      <c r="X18" s="8" t="s">
+      <c r="AB18" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:28">
       <c r="A19" s="6" t="s">
         <v>0</v>
       </c>
@@ -1977,25 +2112,29 @@
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
-      <c r="T19" s="8" t="s">
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U19" s="8" t="s">
+      <c r="Y19" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="V19" s="13">
+      <c r="Z19" s="13">
         <f t="shared" si="3"/>
         <v>1.157407407407407E-7</v>
       </c>
-      <c r="W19" s="13">
+      <c r="AA19" s="13">
         <f t="shared" si="4"/>
         <v>1.157407407407407E-5</v>
       </c>
-      <c r="X19" s="8" t="s">
+      <c r="AB19" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:28">
       <c r="A20" s="6" t="s">
         <v>2</v>
       </c>
@@ -2027,23 +2166,27 @@
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
-      <c r="T20" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="U20" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="V20" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="W20" s="8">
-        <v>0.9</v>
-      </c>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
       <c r="X20" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:24">
+      <c r="Y20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z20" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="AA20" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="AB20" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28">
       <c r="A21" s="6" t="s">
         <v>3</v>
       </c>
@@ -2075,23 +2218,27 @@
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
-      <c r="T21" s="8" t="s">
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U21" s="8" t="s">
+      <c r="Y21" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="V21" s="8">
+      <c r="Z21" s="8">
         <v>0.1</v>
       </c>
-      <c r="W21" s="8">
+      <c r="AA21" s="8">
         <v>0.9</v>
       </c>
-      <c r="X21" s="8" t="s">
+      <c r="AB21" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:28">
       <c r="A22" s="6" t="s">
         <v>4</v>
       </c>
@@ -2123,17 +2270,21 @@
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
       <c r="S22" s="8"/>
-      <c r="T22" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U22" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
       <c r="V22" s="8"/>
       <c r="W22" s="8"/>
-      <c r="X22" s="8"/>
-    </row>
-    <row r="23" spans="1:24">
+      <c r="X22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z22" s="8"/>
+      <c r="AA22" s="8"/>
+      <c r="AB22" s="8"/>
+    </row>
+    <row r="23" spans="1:28">
       <c r="A23" s="6" t="s">
         <v>5</v>
       </c>
@@ -2165,17 +2316,21 @@
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
       <c r="S23" s="8"/>
-      <c r="T23" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U23" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
       <c r="V23" s="8"/>
       <c r="W23" s="8"/>
-      <c r="X23" s="8"/>
-    </row>
-    <row r="24" spans="1:24">
+      <c r="X23" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y23" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z23" s="8"/>
+      <c r="AA23" s="8"/>
+      <c r="AB23" s="8"/>
+    </row>
+    <row r="24" spans="1:28">
       <c r="A24" s="17" t="s">
         <v>62</v>
       </c>
@@ -2207,17 +2362,21 @@
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
       <c r="S24" s="8"/>
-      <c r="T24" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U24" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
       <c r="V24" s="8"/>
       <c r="W24" s="8"/>
-      <c r="X24" s="8"/>
-    </row>
-    <row r="25" spans="1:24">
+      <c r="X24" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y24" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z24" s="8"/>
+      <c r="AA24" s="8"/>
+      <c r="AB24" s="8"/>
+    </row>
+    <row r="25" spans="1:28">
       <c r="A25" s="17" t="s">
         <v>63</v>
       </c>
@@ -2249,17 +2408,21 @@
       <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
-      <c r="T25" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U25" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
       <c r="V25" s="8"/>
       <c r="W25" s="8"/>
-      <c r="X25" s="8"/>
-    </row>
-    <row r="26" spans="1:24">
+      <c r="X25" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y25" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z25" s="8"/>
+      <c r="AA25" s="8"/>
+      <c r="AB25" s="8"/>
+    </row>
+    <row r="26" spans="1:28">
       <c r="A26" s="17" t="s">
         <v>66</v>
       </c>
@@ -2291,17 +2454,21 @@
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
       <c r="S26" s="8"/>
-      <c r="T26" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U26" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
       <c r="V26" s="8"/>
       <c r="W26" s="8"/>
-      <c r="X26" s="8"/>
-    </row>
-    <row r="27" spans="1:24">
+      <c r="X26" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y26" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z26" s="8"/>
+      <c r="AA26" s="8"/>
+      <c r="AB26" s="8"/>
+    </row>
+    <row r="27" spans="1:28">
       <c r="A27" s="17" t="s">
         <v>67</v>
       </c>
@@ -2333,17 +2500,21 @@
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
-      <c r="T27" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U27" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
       <c r="V27" s="8"/>
       <c r="W27" s="8"/>
-      <c r="X27" s="8"/>
-    </row>
-    <row r="28" spans="1:24">
+      <c r="X27" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y27" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z27" s="8"/>
+      <c r="AA27" s="8"/>
+      <c r="AB27" s="8"/>
+    </row>
+    <row r="28" spans="1:28">
       <c r="A28" s="17" t="s">
         <v>56</v>
       </c>
@@ -2378,17 +2549,21 @@
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
-      <c r="T28" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U28" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
       <c r="V28" s="8"/>
       <c r="W28" s="8"/>
-      <c r="X28" s="8"/>
-    </row>
-    <row r="29" spans="1:24">
+      <c r="X28" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y28" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z28" s="8"/>
+      <c r="AA28" s="8"/>
+      <c r="AB28" s="8"/>
+    </row>
+    <row r="29" spans="1:28">
       <c r="A29" s="17" t="s">
         <v>57</v>
       </c>
@@ -2424,17 +2599,21 @@
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
-      <c r="T29" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U29" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="T29" s="8"/>
+      <c r="U29" s="8"/>
       <c r="V29" s="8"/>
       <c r="W29" s="8"/>
-      <c r="X29" s="8"/>
-    </row>
-    <row r="30" spans="1:24">
+      <c r="X29" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y29" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z29" s="8"/>
+      <c r="AA29" s="8"/>
+      <c r="AB29" s="8"/>
+    </row>
+    <row r="30" spans="1:28">
       <c r="A30" s="6" t="s">
         <v>24</v>
       </c>
@@ -2466,17 +2645,21 @@
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
-      <c r="T30" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U30" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
       <c r="V30" s="8"/>
       <c r="W30" s="8"/>
-      <c r="X30" s="8"/>
-    </row>
-    <row r="31" spans="1:24">
+      <c r="X30" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y30" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z30" s="8"/>
+      <c r="AA30" s="8"/>
+      <c r="AB30" s="8"/>
+    </row>
+    <row r="31" spans="1:28">
       <c r="A31" s="6" t="s">
         <v>25</v>
       </c>
@@ -2508,17 +2691,21 @@
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
-      <c r="T31" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U31" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="T31" s="8"/>
+      <c r="U31" s="8"/>
       <c r="V31" s="8"/>
       <c r="W31" s="8"/>
-      <c r="X31" s="8"/>
-    </row>
-    <row r="32" spans="1:24">
+      <c r="X31" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y31" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z31" s="8"/>
+      <c r="AA31" s="8"/>
+      <c r="AB31" s="8"/>
+    </row>
+    <row r="32" spans="1:28">
       <c r="A32" s="6" t="s">
         <v>22</v>
       </c>
@@ -2553,17 +2740,21 @@
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
-      <c r="T32" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U32" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="T32" s="8"/>
+      <c r="U32" s="8"/>
       <c r="V32" s="8"/>
       <c r="W32" s="8"/>
-      <c r="X32" s="8"/>
-    </row>
-    <row r="33" spans="1:24">
+      <c r="X32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z32" s="8"/>
+      <c r="AA32" s="8"/>
+      <c r="AB32" s="8"/>
+    </row>
+    <row r="33" spans="1:28">
       <c r="A33" s="6" t="s">
         <v>23</v>
       </c>
@@ -2598,17 +2789,21 @@
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
-      <c r="T33" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U33" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="T33" s="8"/>
+      <c r="U33" s="8"/>
       <c r="V33" s="8"/>
       <c r="W33" s="8"/>
-      <c r="X33" s="8"/>
-    </row>
-    <row r="34" spans="1:24">
+      <c r="X33" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y33" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z33" s="8"/>
+      <c r="AA33" s="8"/>
+      <c r="AB33" s="8"/>
+    </row>
+    <row r="34" spans="1:28">
       <c r="A34" s="17" t="s">
         <v>87</v>
       </c>
@@ -2644,17 +2839,21 @@
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
-      <c r="T34" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U34" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
       <c r="V34" s="8"/>
       <c r="W34" s="8"/>
-      <c r="X34" s="8"/>
-    </row>
-    <row r="35" spans="1:24">
+      <c r="X34" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y34" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z34" s="8"/>
+      <c r="AA34" s="8"/>
+      <c r="AB34" s="8"/>
+    </row>
+    <row r="35" spans="1:28">
       <c r="A35" s="17" t="s">
         <v>84</v>
       </c>
@@ -2686,17 +2885,21 @@
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
-      <c r="T35" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U35" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="T35" s="8"/>
+      <c r="U35" s="8"/>
       <c r="V35" s="8"/>
       <c r="W35" s="8"/>
-      <c r="X35" s="8"/>
-    </row>
-    <row r="36" spans="1:24">
+      <c r="X35" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y35" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z35" s="8"/>
+      <c r="AA35" s="8"/>
+      <c r="AB35" s="8"/>
+    </row>
+    <row r="36" spans="1:28">
       <c r="A36" s="17" t="s">
         <v>85</v>
       </c>
@@ -2745,25 +2948,31 @@
       <c r="S36" s="8">
         <v>0</v>
       </c>
-      <c r="T36" s="8" t="s">
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="8">
+        <v>0</v>
+      </c>
+      <c r="W36" s="8"/>
+      <c r="X36" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U36" s="8" t="s">
+      <c r="Y36" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="V36" s="13">
+      <c r="Z36" s="13">
         <f>B36/10</f>
         <v>1.1574074074074099E-7</v>
       </c>
-      <c r="W36" s="13">
+      <c r="AA36" s="13">
         <f>B36*10</f>
         <v>1.1574074074074099E-5</v>
       </c>
-      <c r="X36" s="8" t="s">
+      <c r="AB36" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:24">
+    <row r="37" spans="1:28">
       <c r="A37" s="6" t="s">
         <v>68</v>
       </c>
@@ -2819,17 +3028,29 @@
       <c r="S37" s="8">
         <v>1</v>
       </c>
-      <c r="T37" s="8" t="s">
+      <c r="T37" s="8">
+        <v>0</v>
+      </c>
+      <c r="U37" s="8">
+        <v>1</v>
+      </c>
+      <c r="V37" s="8">
+        <v>1</v>
+      </c>
+      <c r="W37" s="8">
+        <v>1</v>
+      </c>
+      <c r="X37" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U37" s="8" t="s">
+      <c r="Y37" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V37" s="8"/>
-      <c r="W37" s="8"/>
-      <c r="X37" s="8"/>
-    </row>
-    <row r="38" spans="1:24">
+      <c r="Z37" s="8"/>
+      <c r="AA37" s="8"/>
+      <c r="AB37" s="8"/>
+    </row>
+    <row r="38" spans="1:28">
       <c r="A38" s="6" t="s">
         <v>88</v>
       </c>
@@ -2878,25 +3099,31 @@
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
-      <c r="T38" s="8" t="s">
+      <c r="T38" s="8">
+        <v>0</v>
+      </c>
+      <c r="U38" s="8"/>
+      <c r="V38" s="8"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U38" s="8" t="s">
+      <c r="Y38" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V38" s="13">
+      <c r="Z38" s="13">
         <f>B38/10</f>
         <v>1.157407407407407E-7</v>
       </c>
-      <c r="W38" s="13">
+      <c r="AA38" s="13">
         <f>B38*10</f>
         <v>1.157407407407407E-5</v>
       </c>
-      <c r="X38" s="8" t="s">
+      <c r="AB38" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:24">
+    <row r="39" spans="1:28">
       <c r="A39" s="6" t="s">
         <v>89</v>
       </c>
@@ -2945,25 +3172,31 @@
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
-      <c r="T39" s="8" t="s">
+      <c r="T39" s="8">
+        <v>0</v>
+      </c>
+      <c r="U39" s="8"/>
+      <c r="V39" s="8"/>
+      <c r="W39" s="8"/>
+      <c r="X39" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U39" s="8" t="s">
+      <c r="Y39" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="V39" s="13">
+      <c r="Z39" s="13">
         <f>B39/10</f>
         <v>1.157407407407407E-7</v>
       </c>
-      <c r="W39" s="13">
+      <c r="AA39" s="13">
         <f>B39*10</f>
         <v>1.157407407407407E-5</v>
       </c>
-      <c r="X39" s="8" t="s">
+      <c r="AB39" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:24">
+    <row r="40" spans="1:28">
       <c r="A40" s="19" t="s">
         <v>69</v>
       </c>
@@ -3019,17 +3252,29 @@
       <c r="S40" s="8">
         <v>1</v>
       </c>
-      <c r="T40" s="8" t="s">
+      <c r="T40" s="8">
+        <v>1</v>
+      </c>
+      <c r="U40" s="8">
+        <v>0</v>
+      </c>
+      <c r="V40" s="8">
+        <v>1</v>
+      </c>
+      <c r="W40" s="8">
+        <v>1</v>
+      </c>
+      <c r="X40" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U40" s="8" t="s">
+      <c r="Y40" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V40" s="8"/>
-      <c r="W40" s="8"/>
-      <c r="X40" s="8"/>
-    </row>
-    <row r="41" spans="1:24">
+      <c r="Z40" s="8"/>
+      <c r="AA40" s="8"/>
+      <c r="AB40" s="8"/>
+    </row>
+    <row r="41" spans="1:28">
       <c r="A41" s="6" t="s">
         <v>100</v>
       </c>
@@ -3078,25 +3323,31 @@
         <v>0</v>
       </c>
       <c r="S41" s="8"/>
-      <c r="T41" s="8" t="s">
+      <c r="T41" s="8"/>
+      <c r="U41" s="8">
+        <v>0</v>
+      </c>
+      <c r="V41" s="8"/>
+      <c r="W41" s="8"/>
+      <c r="X41" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U41" s="8" t="s">
+      <c r="Y41" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V41" s="13">
+      <c r="Z41" s="13">
         <f>B41/10</f>
         <v>4.6960167714884693E-10</v>
       </c>
-      <c r="W41" s="13">
+      <c r="AA41" s="13">
         <f>B41*10</f>
         <v>4.6960167714884692E-8</v>
       </c>
-      <c r="X41" s="8" t="s">
+      <c r="AB41" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:24">
+    <row r="42" spans="1:28">
       <c r="A42" s="6" t="s">
         <v>101</v>
       </c>
@@ -3145,25 +3396,31 @@
         <v>0</v>
       </c>
       <c r="S42" s="8"/>
-      <c r="T42" s="8" t="s">
+      <c r="T42" s="8"/>
+      <c r="U42" s="8">
+        <v>0</v>
+      </c>
+      <c r="V42" s="8"/>
+      <c r="W42" s="8"/>
+      <c r="X42" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U42" s="8" t="s">
+      <c r="Y42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="V42" s="13">
+      <c r="Z42" s="13">
         <f>B42/10</f>
         <v>1.9444444444444442E-9</v>
       </c>
-      <c r="W42" s="13">
+      <c r="AA42" s="13">
         <f>B42*10</f>
         <v>1.9444444444444442E-7</v>
       </c>
-      <c r="X42" s="8" t="s">
+      <c r="AB42" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:24">
+    <row r="43" spans="1:28">
       <c r="A43" s="6" t="s">
         <v>102</v>
       </c>
@@ -3212,25 +3469,31 @@
         <v>0</v>
       </c>
       <c r="S43" s="8"/>
-      <c r="T43" s="8" t="s">
+      <c r="T43" s="8"/>
+      <c r="U43" s="8">
+        <v>0</v>
+      </c>
+      <c r="V43" s="8"/>
+      <c r="W43" s="8"/>
+      <c r="X43" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U43" s="8" t="s">
+      <c r="Y43" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V43" s="13">
+      <c r="Z43" s="13">
         <f>B43/10</f>
         <v>1.9566736547868619E-7</v>
       </c>
-      <c r="W43" s="13">
+      <c r="AA43" s="13">
         <f>B43*10</f>
         <v>1.956673654786862E-5</v>
       </c>
-      <c r="X43" s="8" t="s">
+      <c r="AB43" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:24">
+    <row r="44" spans="1:28">
       <c r="A44" s="6" t="s">
         <v>103</v>
       </c>
@@ -3279,25 +3542,31 @@
         <v>0</v>
       </c>
       <c r="S44" s="8"/>
-      <c r="T44" s="8" t="s">
+      <c r="T44" s="8"/>
+      <c r="U44" s="8">
+        <v>0</v>
+      </c>
+      <c r="V44" s="8"/>
+      <c r="W44" s="8"/>
+      <c r="X44" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U44" s="8" t="s">
+      <c r="Y44" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="V44" s="13">
+      <c r="Z44" s="13">
         <f>B44/10</f>
         <v>9.7222222222222218E-7</v>
       </c>
-      <c r="W44" s="13">
+      <c r="AA44" s="13">
         <f>B44*10</f>
         <v>9.722222222222223E-5</v>
       </c>
-      <c r="X44" s="8" t="s">
+      <c r="AB44" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:24">
+    <row r="45" spans="1:28">
       <c r="A45" s="17" t="s">
         <v>105</v>
       </c>
@@ -3346,17 +3615,23 @@
         <v>0</v>
       </c>
       <c r="S45" s="8"/>
-      <c r="T45" s="8" t="s">
+      <c r="T45" s="8"/>
+      <c r="U45" s="8">
+        <v>0</v>
+      </c>
+      <c r="V45" s="8"/>
+      <c r="W45" s="8"/>
+      <c r="X45" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U45" s="8" t="s">
+      <c r="Y45" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V45" s="13"/>
-      <c r="W45" s="13"/>
-      <c r="X45" s="8"/>
-    </row>
-    <row r="46" spans="1:24" ht="15.75" thickBot="1">
+      <c r="Z45" s="13"/>
+      <c r="AA45" s="13"/>
+      <c r="AB45" s="8"/>
+    </row>
+    <row r="46" spans="1:28" ht="15.75" thickBot="1">
       <c r="A46" s="6" t="s">
         <v>71</v>
       </c>
@@ -3402,25 +3677,31 @@
         <v>0</v>
       </c>
       <c r="S46" s="8"/>
-      <c r="T46" s="8" t="s">
+      <c r="T46" s="8"/>
+      <c r="U46" s="8">
+        <v>0</v>
+      </c>
+      <c r="V46" s="8"/>
+      <c r="W46" s="8"/>
+      <c r="X46" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U46" s="8" t="s">
+      <c r="Y46" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V46" s="13">
+      <c r="Z46" s="13">
         <f>B46/10</f>
         <v>3.4055555555555557E-6</v>
       </c>
-      <c r="W46" s="13">
+      <c r="AA46" s="13">
         <f>B46*10</f>
         <v>3.4055555555555559E-4</v>
       </c>
-      <c r="X46" s="8" t="s">
+      <c r="AB46" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:24">
+    <row r="47" spans="1:28">
       <c r="A47" s="6" t="s">
         <v>72</v>
       </c>
@@ -3466,25 +3747,31 @@
         <v>0</v>
       </c>
       <c r="S47" s="8"/>
-      <c r="T47" s="8" t="s">
+      <c r="T47" s="8"/>
+      <c r="U47" s="8">
+        <v>0</v>
+      </c>
+      <c r="V47" s="8"/>
+      <c r="W47" s="8"/>
+      <c r="X47" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U47" s="8" t="s">
+      <c r="Y47" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="V47" s="13">
+      <c r="Z47" s="13">
         <f>B47/10</f>
         <v>3.4055555555555561E-9</v>
       </c>
-      <c r="W47" s="13">
+      <c r="AA47" s="13">
         <f>B47*10</f>
         <v>3.4055555555555562E-7</v>
       </c>
-      <c r="X47" s="8" t="s">
+      <c r="AB47" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:24">
+    <row r="48" spans="1:28">
       <c r="A48" s="2" t="s">
         <v>114</v>
       </c>
@@ -3526,16 +3813,22 @@
         <v>0</v>
       </c>
       <c r="S48" s="20"/>
-      <c r="T48" s="20" t="s">
+      <c r="T48" s="20"/>
+      <c r="U48" s="20">
+        <v>0</v>
+      </c>
+      <c r="V48" s="20"/>
+      <c r="W48" s="20"/>
+      <c r="X48" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="U48" s="20" t="s">
+      <c r="Y48" s="20" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X48" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A39:X40">
+  <autoFilter ref="A1:AB48" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A39:AB40">
       <sortCondition ref="A1:A47"/>
     </sortState>
   </autoFilter>
@@ -3613,93 +3906,141 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59EF6688-3E5C-4F06-8A01-A83A75DD0983}">
-  <dimension ref="A1:A16384"/>
+  <dimension ref="A1:E16384"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A19"/>
+      <selection activeCell="E13" sqref="E13:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5">
       <c r="A1" s="17"/>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="E1" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="23"/>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="E2" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="17"/>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="E3" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="24"/>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="E4" s="25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="17"/>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="E5" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="17"/>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="E6" s="25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="17"/>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="E7" s="25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="25" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
+        <v>115</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="25" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="E9" s="25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="25" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="E10" s="25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="25" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="E11" s="25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="25" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="E12" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="25" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
+        <v>116</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="25" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
+        <v>117</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="25" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
+        <v>118</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="25" t="s">
-        <v>126</v>
+        <v>119</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="25" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="25" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="25" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:1">

</xml_diff>